<commit_message>
solved Moq - Advanced Interview Questions
</commit_message>
<xml_diff>
--- a/src/UnitTesting - Advanced - Moq/CRUDExample/wwwroot/templates/countries_template.xlsx
+++ b/src/UnitTesting - Advanced - Moq/CRUDExample/wwwroot/templates/countries_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\source\repos\ASPNETCore7\ASPNETCore7\src\EntityFramework\CRUDExample\wwwroot\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\source\repos\ASPNETCore7\ASPNETCore7\src\UnitTesting - Advanced - Moq\CRUDExample\wwwroot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0222383E-66D1-41EA-A590-6782B1A3BFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB16DA3A-E954-4231-B047-CC0AEDC980E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5145" yWindow="2970" windowWidth="21600" windowHeight="11295" xr2:uid="{B1F2AF36-6242-43EB-8347-2E7070823BB4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>CountryName</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>ghi</t>
+  </si>
+  <si>
+    <t>jona</t>
   </si>
 </sst>
 </file>
@@ -72,8 +75,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF95112E-FBB5-41A6-A6E3-5F6411C87CCE}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,6 +420,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>